<commit_message>
Updated cluster typology Excel
</commit_message>
<xml_diff>
--- a/Results/Cluster_analysis/k_means/provinces_clusters.xlsx
+++ b/Results/Cluster_analysis/k_means/provinces_clusters.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt&amp;Kez\Documents\Matt PhD\PhD_Chapter1\Results\Cluster_analysis\k_means\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A913FF71-7CAD-4E28-AA08-1039F606D6E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C242E9-D5F3-4429-AEF3-889ECBF56AE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="provinces_clusters" sheetId="1" r:id="rId1"/>
     <sheet name="groups" sheetId="2" r:id="rId2"/>
+    <sheet name="Broader typology" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>Banteay Meanchey</t>
   </si>
@@ -110,9 +111,6 @@
     <t>sec</t>
   </si>
   <si>
-    <t>rural livelihoods</t>
-  </si>
-  <si>
     <t>access to serv</t>
   </si>
   <si>
@@ -123,12 +121,48 @@
   </si>
   <si>
     <t>migration</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Clusters</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Rural 1</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>Forest cover</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>Rural 2</t>
+  </si>
+  <si>
+    <t>6, 8</t>
+  </si>
+  <si>
+    <t>Econ_securtiy via rural livelihoods</t>
+  </si>
+  <si>
+    <t>Very low levels of education, predominantly primary sector employment, majority of population reliant on rural/agricultural livelhoods for economic security, poor access to services, higher levels of crime per capita, low levels of land conflict, low levels of in- and out-migration</t>
+  </si>
+  <si>
+    <t>Generally low levels of education, predominantly primary sector employment, majority of population not reliant on rural liveihoods for economic security, better access to services than Rural1 group, very low criminality per capita but very high rates of land conflict, and high levels of in- and out-migration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -265,7 +299,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,6 +477,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -606,11 +652,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -965,7 +1017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1097,43 +1149,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
     <col min="12" max="12" width="4.140625" customWidth="1"/>
     <col min="15" max="15" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>31</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>32</v>
-      </c>
-      <c r="S1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1181,25 +1234,25 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>1</v>
       </c>
       <c r="E3">
         <v>4</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <v>1</v>
       </c>
       <c r="H3">
         <v>5</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="4">
         <v>1</v>
       </c>
       <c r="K3">
@@ -1208,16 +1261,16 @@
       <c r="M3">
         <v>3</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="4">
         <v>1</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="4">
         <v>1</v>
       </c>
       <c r="Q3">
         <v>3</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="4">
         <v>1</v>
       </c>
       <c r="T3">
@@ -1225,25 +1278,25 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>2</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="5">
         <v>6</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="4">
         <v>2</v>
       </c>
       <c r="K4">
@@ -1252,16 +1305,16 @@
       <c r="M4">
         <v>5</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="4">
         <v>2</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="4">
         <v>2</v>
       </c>
       <c r="Q4">
         <v>5</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="4">
         <v>2</v>
       </c>
       <c r="T4">
@@ -1269,22 +1322,22 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="5">
         <v>6</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>6</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <v>8</v>
       </c>
       <c r="K5">
         <v>5</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="5">
         <v>6</v>
       </c>
       <c r="N5">
@@ -1293,27 +1346,30 @@
       <c r="P5">
         <v>4</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="5">
         <v>6</v>
       </c>
       <c r="S5">
         <v>4</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D6">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5">
         <v>8</v>
       </c>
       <c r="G6">
         <v>4</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="5">
         <v>6</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="5">
         <v>8</v>
       </c>
       <c r="N6">
@@ -1322,13 +1378,13 @@
       <c r="P6">
         <v>7</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="5">
         <v>8</v>
       </c>
       <c r="S6">
         <v>7</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="5">
         <v>8</v>
       </c>
     </row>
@@ -1350,7 +1406,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K8">
+      <c r="K8" s="5">
         <v>8</v>
       </c>
     </row>
@@ -1362,4 +1418,64 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04DD17F-A1AF-4853-9552-4B51037E02F2}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="110.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
re-doing the group typology using quantile heatmap
</commit_message>
<xml_diff>
--- a/Results/Cluster_analysis/k_means/provinces_clusters.xlsx
+++ b/Results/Cluster_analysis/k_means/provinces_clusters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt&amp;Kez\Documents\Matt PhD\PhD_Chapter1\Results\Cluster_analysis\k_means\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C242E9-D5F3-4429-AEF3-889ECBF56AE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3E27AE-68B9-4D19-91F8-941C2BAFD337}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-2130" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="provinces_clusters" sheetId="1" r:id="rId1"/>
@@ -299,7 +299,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -477,18 +477,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -652,7 +640,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -661,8 +649,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1150,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,7 +1153,7 @@
     <col min="15" max="15" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1189,7 +1176,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1233,187 +1220,204 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
+      <c r="B3" s="4">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4"/>
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="E3" s="4">
         <v>1</v>
       </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="J3" s="4">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="M3">
-        <v>3</v>
-      </c>
-      <c r="N3" s="4">
-        <v>1</v>
-      </c>
-      <c r="P3" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>3</v>
-      </c>
-      <c r="S3" s="4">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
+      <c r="B4" s="4">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="4">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4">
         <v>5</v>
       </c>
-      <c r="G4" s="4">
-        <v>2</v>
-      </c>
-      <c r="H4" s="5">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4">
         <v>6</v>
       </c>
-      <c r="J4" s="4">
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <v>4</v>
-      </c>
-      <c r="M4">
-        <v>5</v>
-      </c>
-      <c r="N4" s="4">
-        <v>2</v>
-      </c>
-      <c r="P4" s="4">
-        <v>2</v>
-      </c>
-      <c r="Q4">
-        <v>5</v>
-      </c>
-      <c r="S4" s="4">
-        <v>2</v>
-      </c>
-      <c r="T4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5">
-        <v>6</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5" s="5">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4">
         <v>8</v>
       </c>
-      <c r="K5">
-        <v>5</v>
-      </c>
-      <c r="M5" s="5">
-        <v>6</v>
-      </c>
-      <c r="N5">
-        <v>4</v>
-      </c>
-      <c r="P5">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>6</v>
-      </c>
-      <c r="S5">
-        <v>4</v>
-      </c>
-      <c r="T5" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5">
-        <v>8</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="K6" s="5">
-        <v>6</v>
-      </c>
-      <c r="M6" s="5">
-        <v>8</v>
-      </c>
-      <c r="N6">
-        <v>7</v>
-      </c>
-      <c r="P6">
-        <v>7</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>8</v>
-      </c>
-      <c r="S6">
-        <v>7</v>
-      </c>
-      <c r="T6" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D7">
-        <v>9</v>
-      </c>
-      <c r="K7">
-        <v>7</v>
-      </c>
-      <c r="M7">
-        <v>9</v>
-      </c>
-      <c r="P7">
-        <v>9</v>
-      </c>
-      <c r="S7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K8" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K9">
-        <v>9</v>
-      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
starting to UPGMA typology
</commit_message>
<xml_diff>
--- a/Results/Cluster_analysis/k_means/provinces_clusters.xlsx
+++ b/Results/Cluster_analysis/k_means/provinces_clusters.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Results\Cluster_analysis\k_means\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D6C1C6-586F-4E93-B77B-519AF45B8CC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8757E891-1B64-4E07-AA0D-0DADB7113E51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="provinces_clusters" sheetId="1" r:id="rId1"/>
     <sheet name="groups" sheetId="2" r:id="rId2"/>
     <sheet name="Broader typology_kmeans" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
+    <sheet name="broader typology_UPGMA" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>Banteay Meanchey</t>
   </si>
@@ -174,9 +176,6 @@
     <t>RANGE: VERY HIGH TO VERY LOW</t>
   </si>
   <si>
-    <t>Unk 3</t>
-  </si>
-  <si>
     <t>4, 5</t>
   </si>
   <si>
@@ -195,9 +194,6 @@
     <t>3,7,9</t>
   </si>
   <si>
-    <t>Unk 4</t>
-  </si>
-  <si>
     <t>Mostly lower elevation provinces that range in size. Mostly lower proportions of primary sector workers but always relatively high proportions of secondary sector workers. Generally lower levels of farmland but higher proportions of livestock. Range of access to services, the majority being high.  Range of criminality levels, the majority being high. Mostly high levels of migration and land conflict</t>
   </si>
   <si>
@@ -205,6 +201,15 @@
   </si>
   <si>
     <t>RANGE: LOW TO HIGH</t>
+  </si>
+  <si>
+    <t>Cluster</t>
+  </si>
+  <si>
+    <t>Urban 1</t>
+  </si>
+  <si>
+    <t>Urban 2</t>
   </si>
 </sst>
 </file>
@@ -1228,8 +1233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1702,16 +1707,16 @@
     </row>
     <row r="18" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" t="s">
         <v>54</v>
       </c>
-      <c r="J18" t="s">
-        <v>53</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>55</v>
-      </c>
-      <c r="L18" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="19" spans="9:12" x14ac:dyDescent="0.3">
@@ -1743,8 +1748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04DD17F-A1AF-4853-9552-4B51037E02F2}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1798,34 +1803,354 @@
     </row>
     <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
         <v>50</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" t="s">
         <v>58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12FE6095-4C7D-48E0-A4E0-36D61AB3DF88}">
+  <dimension ref="A1:X6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="2.88671875" customWidth="1"/>
+    <col min="8" max="8" width="2" customWidth="1"/>
+    <col min="13" max="13" width="1.6640625" customWidth="1"/>
+    <col min="16" max="16" width="1.21875" customWidth="1"/>
+    <col min="19" max="19" width="1.6640625" customWidth="1"/>
+    <col min="22" max="22" width="2.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="I1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="I2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="11"/>
+      <c r="K2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="10"/>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U3" t="s">
+        <v>25</v>
+      </c>
+      <c r="W3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>3</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="W5">
+        <v>2</v>
+      </c>
+      <c r="X5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>5</v>
+      </c>
+      <c r="U6">
+        <v>5</v>
+      </c>
+      <c r="X6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C63902A-F6B8-48A7-85BE-2E871FB71727}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="53.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Typology using UPGMA done
</commit_message>
<xml_diff>
--- a/Results/Cluster_analysis/k_means/provinces_clusters.xlsx
+++ b/Results/Cluster_analysis/k_means/provinces_clusters.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Results\Cluster_analysis\k_means\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8757E891-1B64-4E07-AA0D-0DADB7113E51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2D593F-B6D6-442A-9B8A-A8EEFFD8B371}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="provinces_clusters" sheetId="1" r:id="rId1"/>
     <sheet name="groups" sheetId="2" r:id="rId2"/>
     <sheet name="Broader typology_kmeans" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
+    <sheet name="groups_UPGMA" sheetId="5" r:id="rId4"/>
     <sheet name="broader typology_UPGMA" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
   <si>
     <t>Banteay Meanchey</t>
   </si>
@@ -210,6 +210,30 @@
   </si>
   <si>
     <t>Urban 2</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>VERY LOW</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>Small provinces at very low elevations. Very high levels of education, high proportion of people in the primary sector, but very high proportion of people in the secondary sector. High proportion of people with no farmland, but high levels of livestock ownership. High access to services and low crime per capita. But very high migration levels and very high rates of land conflict.</t>
+  </si>
+  <si>
+    <t>Large provinces at low elevations. Very high levels of education, and relatively low proportion of workers in the primary and secondary sectors (suggesting higher proportions in the other sectors e.g. tertiary). High proportion of people with no farmland, and low levels of livestock ownership (suggesting very urban).  Low access to services, but this may be explained by the mean size of the provinces in this cluster (there is high access to garbage collection). Low crime per capita, but very high migration and very high rates of land conflict</t>
+  </si>
+  <si>
+    <t>Very large provinces at very high elevations. Very low education levels, very high proportion of primary sector workers and very low proportion of scondary sector workers. Economic security provided by rural livelihoods - few people have no farmland and livestock ownership is common. Very low access to services, high crime per capita, low land conflict and very low migration levels.</t>
+  </si>
+  <si>
+    <t>Very small provinces at very high elevations. Low levels of education, low proportion of people in the primary sector but higher proportion of people in the secondary sector. Very few people with no farmland, but very little livestock ownership. High access to services and high crime per capita. Low land conflict and low migration.</t>
+  </si>
+  <si>
+    <t>Very large provinces at high elevations. High levels of education, and a high proportion of workers in both primary and secondary sectors. Very high proportion of people with no farmland, but also very high proportion of people with livestock. Low access to services (although very high access to garbage collection) - this may be an artefact of the very large mean area of the provinces in this cluster. Very high crime rates, very high migration, and very high rates of land conflict.</t>
   </si>
 </sst>
 </file>
@@ -1839,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12FE6095-4C7D-48E0-A4E0-36D61AB3DF88}">
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2103,14 +2127,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C63902A-F6B8-48A7-85BE-2E871FB71727}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="53.44140625" customWidth="1"/>
+    <col min="2" max="2" width="128.21875" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2125,29 +2149,59 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor edits to the cluster spreadsheet
</commit_message>
<xml_diff>
--- a/Results/Cluster_analysis/k_means/provinces_clusters.xlsx
+++ b/Results/Cluster_analysis/k_means/provinces_clusters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Results\Cluster_analysis\k_means\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B49EC2-41D2-4C72-805E-98081B8319E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F94FD78-F554-48D5-B689-6A7DA3954BC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="778" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -786,12 +786,6 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -800,6 +794,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1310,30 +1310,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="I2" s="11" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="I2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="10" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="10"/>
+      <c r="L2" s="13"/>
       <c r="N2" t="s">
         <v>27</v>
       </c>
@@ -1911,30 +1911,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="I2" s="11" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="I2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="10" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="10"/>
+      <c r="L2" s="13"/>
       <c r="N2" t="s">
         <v>27</v>
       </c>
@@ -2161,7 +2161,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2174,13 +2174,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>71</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -2191,10 +2191,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="11">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2208,10 +2208,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
-        <v>2</v>
-      </c>
-      <c r="B3" s="13">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
         <v>4</v>
       </c>
       <c r="C3" t="s">
@@ -2225,10 +2225,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2242,10 +2242,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="11">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -2259,16 +2259,16 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>76</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>68</v>
       </c>
       <c r="E6" t="s">

</xml_diff>